<commit_message>
Add PlantLine col.  sector 12 changes
</commit_message>
<xml_diff>
--- a/Race Dashboard data/Nominations Category Scoring.xlsx
+++ b/Race Dashboard data/Nominations Category Scoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\McLaren2021\Sanofi\Race Dashboard data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC93361-C042-43B1-BB62-4060DE0EC601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF73CF71-C673-453F-A61F-E3C37B966BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8220" yWindow="825" windowWidth="21600" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List of sites" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="67">
   <si>
     <t>Asset Efficiency Dashboard</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Number of stoppages</t>
+  </si>
+  <si>
+    <t>Better Together</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -460,6 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,7 +473,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,14 +808,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1119,11 +1128,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,9 +1147,10 @@
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -1171,8 +1181,11 @@
       <c r="J1" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>44325</v>
       </c>
@@ -1192,7 +1205,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
@@ -1209,7 +1222,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
@@ -1222,7 +1235,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
@@ -1235,7 +1248,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>28</v>
       </c>
@@ -1254,7 +1267,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>28</v>
       </c>
@@ -1273,7 +1286,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
@@ -1286,7 +1299,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>34</v>
       </c>
@@ -1299,7 +1312,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>40</v>
       </c>
@@ -1312,7 +1325,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>40</v>
       </c>
@@ -1325,7 +1338,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>44</v>
       </c>
@@ -1338,7 +1351,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>44</v>
       </c>
@@ -1351,7 +1364,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>44</v>
       </c>
@@ -1366,7 +1379,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>44</v>
       </c>
@@ -1381,7 +1394,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>44</v>
       </c>
@@ -1628,53 +1641,62 @@
       <c r="G32" s="2"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D33" s="33"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="4"/>
+      <c r="D35" s="34"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="34">
         <v>123</v>
       </c>
       <c r="E36" s="4"/>
@@ -1684,21 +1706,23 @@
       <c r="G36" s="4">
         <v>72</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="4">
         <v>110</v>
       </c>
-      <c r="J36">
+      <c r="I36" s="4"/>
+      <c r="J36" s="4">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="34">
         <v>123</v>
       </c>
       <c r="E37" s="4"/>
@@ -1708,37 +1732,41 @@
       <c r="G37" s="4">
         <v>72</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="4">
         <v>110</v>
       </c>
-      <c r="J37">
+      <c r="I37" s="4"/>
+      <c r="J37" s="4">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="4"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="J38">
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4">
         <v>103</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="34">
         <v>85</v>
       </c>
       <c r="E39" s="4">
@@ -1746,48 +1774,55 @@
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="5"/>
-      <c r="I39">
+      <c r="H39" s="4"/>
+      <c r="I39" s="4">
         <v>88</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="4">
         <v>90</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="4"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="4"/>
+      <c r="D41" s="34"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="34">
         <v>100</v>
       </c>
       <c r="E42" s="4"/>
@@ -1795,18 +1830,21 @@
       <c r="G42" s="4">
         <v>108</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="4">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="34">
         <v>100</v>
       </c>
       <c r="E43" s="4"/>
@@ -1814,444 +1852,606 @@
       <c r="G43" s="4">
         <v>108</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H43" s="4">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="4"/>
+      <c r="D44" s="34"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="4"/>
+      <c r="D45" s="34"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="26"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="6"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="25">
         <v>44423</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="34">
+        <v>87</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4">
+        <v>103</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D48" s="4"/>
+      <c r="D48" s="34"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="4"/>
+      <c r="I48" s="4">
+        <v>103</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="4"/>
+      <c r="D49" s="34"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="4"/>
+      <c r="D50" s="34"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="4"/>
+      <c r="D51" s="34">
+        <v>85</v>
+      </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H51" s="4"/>
+      <c r="I51" s="4">
+        <v>73</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="4"/>
+      <c r="D52" s="34">
+        <v>85</v>
+      </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H52" s="4"/>
+      <c r="I52" s="4">
+        <v>73</v>
+      </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="4"/>
+      <c r="D53" s="34"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="4">
+        <v>95</v>
+      </c>
       <c r="G53" s="4"/>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="4"/>
+      <c r="D54" s="34">
+        <v>100</v>
+      </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="4">
+        <v>96</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4">
+        <v>79</v>
+      </c>
+      <c r="K54" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D55" s="4"/>
+      <c r="D55" s="34"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D56" s="4"/>
+      <c r="D56" s="34"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="4">
+        <v>92</v>
+      </c>
       <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G57" s="4">
+        <v>71</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="5">
+        <f>82+104</f>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D58" s="4"/>
+      <c r="D58" s="34">
+        <v>95</v>
+      </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G58" s="4">
+        <v>71</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="5">
+        <f>82+104</f>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D59" s="4"/>
+      <c r="D59" s="34">
+        <v>89</v>
+      </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
-      <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D60" s="4"/>
+      <c r="D60" s="34">
+        <v>89</v>
+      </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61" s="34">
+        <v>89</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="25">
         <v>44451</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="33"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="4"/>
+      <c r="D63" s="34"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
-      <c r="H63" s="5"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="4"/>
+      <c r="D64" s="34"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="4"/>
+      <c r="D65" s="34"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="5"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="4"/>
+      <c r="D66" s="34"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
-      <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="4"/>
+      <c r="D67" s="34"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
-      <c r="H67" s="5"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D68" s="4"/>
+      <c r="D68" s="34"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="4"/>
+      <c r="D69" s="34"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
-      <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="5"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D70" s="4"/>
+      <c r="D70" s="34"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
-      <c r="H70" s="5"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D71" s="4"/>
+      <c r="D71" s="34"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
-      <c r="H71" s="5"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="D72" s="4"/>
+      <c r="D72" s="34"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
-      <c r="H72" s="5"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D73" s="4"/>
+      <c r="D73" s="34"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
-      <c r="H73" s="5"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D74" s="4"/>
+      <c r="D74" s="34"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="5"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D75" s="4"/>
+      <c r="D75" s="34"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
-      <c r="H75" s="5"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D76" s="6"/>
+      <c r="D76" s="35"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="7"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2261,15 +2461,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B229BFF5554C594B82E9FC809174EC42" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="86981ce8ecfee4f8cc0f2adb451b875d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8b775167-8204-443f-8b29-59fd47cba222" xmlns:ns3="b3794557-cec4-471c-93c9-c2c60a650af6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35c08955053a06b32b015a614aed9775" ns2:_="" ns3:_="">
     <xsd:import namespace="8b775167-8204-443f-8b29-59fd47cba222"/>
@@ -2492,6 +2683,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2537,14 +2737,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5515C04C-B890-4AC7-8FF4-539EF279E5A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9AD12F5-A5FE-4D65-8912-992DA4ED88DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2563,6 +2755,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5515C04C-B890-4AC7-8FF4-539EF279E5A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C01A9AA5-43B7-41B8-9121-3B72524F75AA}">
   <ds:schemaRefs>

</xml_diff>